<commit_message>
chore: change jira to evm
</commit_message>
<xml_diff>
--- a/mock_data.xlsx
+++ b/mock_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamyaolian/Documents/work/skill/cs/job-hunting/portfolio/jira/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D51EC27A-C231-CF4F-A501-CC0CEC0B13B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD7278A-FC29-2340-A83C-E47F964E475F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="540" yWindow="1820" windowWidth="27240" windowHeight="15940" xr2:uid="{BD8936AC-4962-D04D-BE2A-F14B85FF9286}"/>
   </bookViews>
@@ -494,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF4BF895-60DF-B144-9EFC-64CA53C012CD}">
   <dimension ref="A1:Z33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I6" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19:Z33"/>
+    <sheetView tabSelected="1" topLeftCell="C9" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1477,812 +1477,812 @@
     </row>
     <row r="19" spans="14:26" x14ac:dyDescent="0.2">
       <c r="N19" t="str">
-        <f>A1&amp;":'"&amp;N1&amp;"'"</f>
-        <v>task:'Master Service Agreement (MSA)'</v>
+        <f>$A1&amp;":'"&amp;N1&amp;"',"</f>
+        <v>task:'Master Service Agreement (MSA)',</v>
       </c>
       <c r="O19" t="str">
-        <f t="shared" ref="O19:Z29" si="6">B1&amp;":'"&amp;O1&amp;"'"</f>
-        <v>Task:'Statement of Work (SOW)'</v>
+        <f t="shared" ref="O19:Z19" si="6">$A1&amp;":'"&amp;O1&amp;"',"</f>
+        <v>task:'Statement of Work (SOW)',</v>
       </c>
       <c r="P19" t="str">
         <f t="shared" si="6"/>
-        <v>title: 'Task',:'Project Charter'</v>
+        <v>task:'Project Charter',</v>
       </c>
       <c r="Q19" t="str">
         <f t="shared" si="6"/>
-        <v>dataIndex: 'task',:'Project Kick-off'</v>
+        <v>task:'Project Kick-off',</v>
       </c>
       <c r="R19" t="str">
         <f t="shared" si="6"/>
-        <v>key: 'task':'Project Kick-off Deck'</v>
+        <v>task:'Project Kick-off Deck',</v>
       </c>
       <c r="S19" t="str">
         <f t="shared" si="6"/>
-        <v>{title: 'Task',dataIndex: 'task',key: 'task'},:'Pre Kick-off Meeting'</v>
+        <v>task:'Pre Kick-off Meeting',</v>
       </c>
       <c r="T19" t="str">
         <f t="shared" si="6"/>
-        <v>:'Kick-off Meeting'</v>
+        <v>task:'Kick-off Meeting',</v>
       </c>
       <c r="U19" t="str">
         <f t="shared" si="6"/>
-        <v>:'Request for Quote (RFQ)'</v>
+        <v>task:'Request for Quote (RFQ)',</v>
       </c>
       <c r="V19" t="str">
         <f t="shared" si="6"/>
-        <v>:'Project Plan'</v>
+        <v>task:'Project Plan',</v>
       </c>
       <c r="W19" t="str">
         <f t="shared" si="6"/>
-        <v>abc:'Sample Provider Options'</v>
+        <v>task:'Sample Provider Options',</v>
       </c>
       <c r="X19" t="str">
         <f t="shared" si="6"/>
-        <v>:'Procurement Planning'</v>
+        <v>task:'Procurement Planning',</v>
       </c>
       <c r="Y19" t="str">
         <f t="shared" si="6"/>
-        <v>:'Need Analysis'</v>
+        <v>task:'Need Analysis',</v>
       </c>
       <c r="Z19" t="str">
         <f t="shared" si="6"/>
-        <v>:'Sample/Panel Providers'</v>
+        <v>task:'Sample/Panel Providers',</v>
       </c>
     </row>
     <row r="20" spans="14:26" x14ac:dyDescent="0.2">
       <c r="N20" t="str">
-        <f t="shared" ref="N20:N34" si="7">A2&amp;":'"&amp;N2&amp;"'"</f>
-        <v>bac:'2323.8'</v>
+        <f t="shared" ref="N20:Z33" si="7">$A2&amp;":'"&amp;N2&amp;"',"</f>
+        <v>bac:'2323.8',</v>
       </c>
       <c r="O20" t="str">
-        <f t="shared" si="6"/>
-        <v>BAC:'1987.2'</v>
+        <f t="shared" si="7"/>
+        <v>bac:'1987.2',</v>
       </c>
       <c r="P20" t="str">
-        <f t="shared" si="6"/>
-        <v>title: 'BAC',:'2728.1'</v>
+        <f t="shared" si="7"/>
+        <v>bac:'2728.1',</v>
       </c>
       <c r="Q20" t="str">
-        <f t="shared" si="6"/>
-        <v>dataIndex: 'bac',:'942.8'</v>
+        <f t="shared" si="7"/>
+        <v>bac:'942.8',</v>
       </c>
       <c r="R20" t="str">
-        <f t="shared" si="6"/>
-        <v>key: 'bac':'2288.8'</v>
+        <f t="shared" si="7"/>
+        <v>bac:'2288.8',</v>
       </c>
       <c r="S20" t="str">
-        <f t="shared" si="6"/>
-        <v>{title: 'BAC',dataIndex: 'bac',key: 'bac'},:'1710.9'</v>
+        <f t="shared" si="7"/>
+        <v>bac:'1710.9',</v>
       </c>
       <c r="T20" t="str">
-        <f t="shared" si="6"/>
-        <v>:'2197.8'</v>
+        <f t="shared" si="7"/>
+        <v>bac:'2197.8',</v>
       </c>
       <c r="U20" t="str">
-        <f t="shared" si="6"/>
-        <v>:'3052.4'</v>
+        <f t="shared" si="7"/>
+        <v>bac:'3052.4',</v>
       </c>
       <c r="V20" t="str">
-        <f t="shared" si="6"/>
-        <v>:'1185.3'</v>
+        <f t="shared" si="7"/>
+        <v>bac:'1185.3',</v>
       </c>
       <c r="W20" t="str">
-        <f t="shared" si="6"/>
-        <v>:'763.1'</v>
+        <f t="shared" si="7"/>
+        <v>bac:'763.1',</v>
       </c>
       <c r="X20" t="str">
-        <f t="shared" si="6"/>
-        <v>:'1827.7'</v>
+        <f t="shared" si="7"/>
+        <v>bac:'1827.7',</v>
       </c>
       <c r="Y20" t="str">
-        <f t="shared" si="6"/>
-        <v>:'2267.3'</v>
+        <f t="shared" si="7"/>
+        <v>bac:'2267.3',</v>
       </c>
       <c r="Z20" t="str">
-        <f t="shared" si="6"/>
-        <v>:'2403.2'</v>
+        <f t="shared" si="7"/>
+        <v>bac:'2403.2',</v>
       </c>
     </row>
     <row r="21" spans="14:26" x14ac:dyDescent="0.2">
       <c r="N21" t="str">
         <f t="shared" si="7"/>
-        <v>pv:'2323.8'</v>
+        <v>pv:'2323.8',</v>
       </c>
       <c r="O21" t="str">
-        <f t="shared" si="6"/>
-        <v>PV:'1987.2'</v>
+        <f t="shared" si="7"/>
+        <v>pv:'1987.2',</v>
       </c>
       <c r="P21" t="str">
-        <f t="shared" si="6"/>
-        <v>title: 'PV',:'2728.1'</v>
+        <f t="shared" si="7"/>
+        <v>pv:'2728.1',</v>
       </c>
       <c r="Q21" t="str">
-        <f t="shared" si="6"/>
-        <v>dataIndex: 'pv',:'942.8'</v>
+        <f t="shared" si="7"/>
+        <v>pv:'942.8',</v>
       </c>
       <c r="R21" t="str">
-        <f t="shared" si="6"/>
-        <v>key: 'pv':'2288.8'</v>
+        <f t="shared" si="7"/>
+        <v>pv:'2288.8',</v>
       </c>
       <c r="S21" t="str">
-        <f t="shared" si="6"/>
-        <v>{title: 'PV',dataIndex: 'pv',key: 'pv'},:'1710.9'</v>
+        <f t="shared" si="7"/>
+        <v>pv:'1710.9',</v>
       </c>
       <c r="T21" t="str">
-        <f t="shared" si="6"/>
-        <v>:'2197.8'</v>
+        <f t="shared" si="7"/>
+        <v>pv:'2197.8',</v>
       </c>
       <c r="U21" t="str">
-        <f t="shared" si="6"/>
-        <v>:'3052.4'</v>
+        <f t="shared" si="7"/>
+        <v>pv:'3052.4',</v>
       </c>
       <c r="V21" t="str">
-        <f t="shared" si="6"/>
-        <v>:'1185.3'</v>
+        <f t="shared" si="7"/>
+        <v>pv:'1185.3',</v>
       </c>
       <c r="W21" t="str">
-        <f t="shared" si="6"/>
-        <v>:'763.1'</v>
+        <f t="shared" si="7"/>
+        <v>pv:'763.1',</v>
       </c>
       <c r="X21" t="str">
-        <f t="shared" si="6"/>
-        <v>:'1827.7'</v>
+        <f t="shared" si="7"/>
+        <v>pv:'1827.7',</v>
       </c>
       <c r="Y21" t="str">
-        <f t="shared" si="6"/>
-        <v>:'2267.3'</v>
+        <f t="shared" si="7"/>
+        <v>pv:'2267.3',</v>
       </c>
       <c r="Z21" t="str">
-        <f t="shared" si="6"/>
-        <v>:'2403.2'</v>
+        <f t="shared" si="7"/>
+        <v>pv:'2403.2',</v>
       </c>
     </row>
     <row r="22" spans="14:26" x14ac:dyDescent="0.2">
       <c r="N22" t="str">
         <f t="shared" si="7"/>
-        <v>ev:'2323.8'</v>
+        <v>ev:'2323.8',</v>
       </c>
       <c r="O22" t="str">
-        <f t="shared" si="6"/>
-        <v>EV:'1987.2'</v>
+        <f t="shared" si="7"/>
+        <v>ev:'1987.2',</v>
       </c>
       <c r="P22" t="str">
-        <f t="shared" si="6"/>
-        <v>title: 'EV',:'2728.1'</v>
+        <f t="shared" si="7"/>
+        <v>ev:'2728.1',</v>
       </c>
       <c r="Q22" t="str">
-        <f t="shared" si="6"/>
-        <v>dataIndex: 'ev',:'942.8'</v>
+        <f t="shared" si="7"/>
+        <v>ev:'942.8',</v>
       </c>
       <c r="R22" t="str">
-        <f t="shared" si="6"/>
-        <v>key: 'ev':'2288.8'</v>
+        <f t="shared" si="7"/>
+        <v>ev:'2288.8',</v>
       </c>
       <c r="S22" t="str">
-        <f t="shared" si="6"/>
-        <v>{title: 'EV',dataIndex: 'ev',key: 'ev'},:'1710.9'</v>
+        <f t="shared" si="7"/>
+        <v>ev:'1710.9',</v>
       </c>
       <c r="T22" t="str">
-        <f t="shared" si="6"/>
-        <v>:'2197.8'</v>
+        <f t="shared" si="7"/>
+        <v>ev:'2197.8',</v>
       </c>
       <c r="U22" t="str">
-        <f t="shared" si="6"/>
-        <v>:'3052.4'</v>
+        <f t="shared" si="7"/>
+        <v>ev:'3052.4',</v>
       </c>
       <c r="V22" t="str">
-        <f t="shared" si="6"/>
-        <v>:'1185.3'</v>
+        <f t="shared" si="7"/>
+        <v>ev:'1185.3',</v>
       </c>
       <c r="W22" t="str">
-        <f t="shared" si="6"/>
-        <v>:'763.1'</v>
+        <f t="shared" si="7"/>
+        <v>ev:'763.1',</v>
       </c>
       <c r="X22" t="str">
-        <f t="shared" si="6"/>
-        <v>:'1827.7'</v>
+        <f t="shared" si="7"/>
+        <v>ev:'1827.7',</v>
       </c>
       <c r="Y22" t="str">
-        <f t="shared" si="6"/>
-        <v>:'2267.3'</v>
+        <f t="shared" si="7"/>
+        <v>ev:'2267.3',</v>
       </c>
       <c r="Z22" t="str">
-        <f t="shared" si="6"/>
-        <v>:'2403.2'</v>
+        <f t="shared" si="7"/>
+        <v>ev:'2403.2',</v>
       </c>
     </row>
     <row r="23" spans="14:26" x14ac:dyDescent="0.2">
       <c r="N23" t="str">
         <f t="shared" si="7"/>
-        <v>ac:'3039.5'</v>
+        <v>ac:'3039.5',</v>
       </c>
       <c r="O23" t="str">
-        <f t="shared" si="6"/>
-        <v>AC:'1778.2'</v>
+        <f t="shared" si="7"/>
+        <v>ac:'1778.2',</v>
       </c>
       <c r="P23" t="str">
-        <f t="shared" si="6"/>
-        <v>title: 'AC',:'1905.5'</v>
+        <f t="shared" si="7"/>
+        <v>ac:'1905.5',</v>
       </c>
       <c r="Q23" t="str">
-        <f t="shared" si="6"/>
-        <v>dataIndex: 'ac',:'1231.2'</v>
+        <f t="shared" si="7"/>
+        <v>ac:'1231.2',</v>
       </c>
       <c r="R23" t="str">
-        <f t="shared" si="6"/>
-        <v>key: 'ac':'1613.5'</v>
+        <f t="shared" si="7"/>
+        <v>ac:'1613.5',</v>
       </c>
       <c r="S23" t="str">
-        <f t="shared" si="6"/>
-        <v>{title: 'AC',dataIndex: 'ac',key: 'ac'},:'2328.8'</v>
+        <f t="shared" si="7"/>
+        <v>ac:'2328.8',</v>
       </c>
       <c r="T23" t="str">
-        <f t="shared" si="6"/>
-        <v>:'1702.1'</v>
+        <f t="shared" si="7"/>
+        <v>ac:'1702.1',</v>
       </c>
       <c r="U23" t="str">
-        <f t="shared" si="6"/>
-        <v>:'3431.6'</v>
+        <f t="shared" si="7"/>
+        <v>ac:'3431.6',</v>
       </c>
       <c r="V23" t="str">
-        <f t="shared" si="6"/>
-        <v>:'721.1'</v>
+        <f t="shared" si="7"/>
+        <v>ac:'721.1',</v>
       </c>
       <c r="W23" t="str">
-        <f t="shared" si="6"/>
-        <v>:'1222'</v>
+        <f t="shared" si="7"/>
+        <v>ac:'1222',</v>
       </c>
       <c r="X23" t="str">
-        <f t="shared" si="6"/>
-        <v>:'1688.5'</v>
+        <f t="shared" si="7"/>
+        <v>ac:'1688.5',</v>
       </c>
       <c r="Y23" t="str">
-        <f t="shared" si="6"/>
-        <v>:'1833.4'</v>
+        <f t="shared" si="7"/>
+        <v>ac:'1833.4',</v>
       </c>
       <c r="Z23" t="str">
-        <f t="shared" si="6"/>
-        <v>:'3036.2'</v>
+        <f t="shared" si="7"/>
+        <v>ac:'3036.2',</v>
       </c>
     </row>
     <row r="24" spans="14:26" x14ac:dyDescent="0.2">
       <c r="N24" t="str">
         <f t="shared" si="7"/>
-        <v>cv:'-715.7'</v>
+        <v>cv:'-715.7',</v>
       </c>
       <c r="O24" t="str">
-        <f t="shared" si="6"/>
-        <v>CV:'209'</v>
+        <f t="shared" si="7"/>
+        <v>cv:'209',</v>
       </c>
       <c r="P24" t="str">
-        <f t="shared" si="6"/>
-        <v>title: 'CV',:'822.6'</v>
+        <f t="shared" si="7"/>
+        <v>cv:'822.6',</v>
       </c>
       <c r="Q24" t="str">
-        <f t="shared" si="6"/>
-        <v>dataIndex: 'cv',:'-288.4'</v>
+        <f t="shared" si="7"/>
+        <v>cv:'-288.4',</v>
       </c>
       <c r="R24" t="str">
-        <f t="shared" si="6"/>
-        <v>key: 'cv':'675.3'</v>
+        <f t="shared" si="7"/>
+        <v>cv:'675.3',</v>
       </c>
       <c r="S24" t="str">
-        <f t="shared" si="6"/>
-        <v>{title: 'CV',dataIndex: 'cv',key: 'cv'},:'-617.9'</v>
+        <f t="shared" si="7"/>
+        <v>cv:'-617.9',</v>
       </c>
       <c r="T24" t="str">
-        <f t="shared" si="6"/>
-        <v>:'495.7'</v>
+        <f t="shared" si="7"/>
+        <v>cv:'495.7',</v>
       </c>
       <c r="U24" t="str">
-        <f t="shared" si="6"/>
-        <v>:'-379.2'</v>
+        <f t="shared" si="7"/>
+        <v>cv:'-379.2',</v>
       </c>
       <c r="V24" t="str">
-        <f t="shared" si="6"/>
-        <v>:'464.2'</v>
+        <f t="shared" si="7"/>
+        <v>cv:'464.2',</v>
       </c>
       <c r="W24" t="str">
-        <f t="shared" si="6"/>
-        <v>:'-458.9'</v>
+        <f t="shared" si="7"/>
+        <v>cv:'-458.9',</v>
       </c>
       <c r="X24" t="str">
-        <f t="shared" si="6"/>
-        <v>:'139.2'</v>
+        <f t="shared" si="7"/>
+        <v>cv:'139.2',</v>
       </c>
       <c r="Y24" t="str">
-        <f t="shared" si="6"/>
-        <v>:'433.9'</v>
+        <f t="shared" si="7"/>
+        <v>cv:'433.9',</v>
       </c>
       <c r="Z24" t="str">
-        <f t="shared" si="6"/>
-        <v>:'-633'</v>
+        <f t="shared" si="7"/>
+        <v>cv:'-633',</v>
       </c>
     </row>
     <row r="25" spans="14:26" x14ac:dyDescent="0.2">
       <c r="N25" t="str">
         <f t="shared" si="7"/>
-        <v>sv:'0'</v>
+        <v>sv:'0',</v>
       </c>
       <c r="O25" t="str">
-        <f t="shared" si="6"/>
-        <v>SV:'0'</v>
+        <f t="shared" si="7"/>
+        <v>sv:'0',</v>
       </c>
       <c r="P25" t="str">
-        <f t="shared" si="6"/>
-        <v>title: 'SV',:'0'</v>
+        <f t="shared" si="7"/>
+        <v>sv:'0',</v>
       </c>
       <c r="Q25" t="str">
-        <f t="shared" si="6"/>
-        <v>dataIndex: 'sv',:'0'</v>
+        <f t="shared" si="7"/>
+        <v>sv:'0',</v>
       </c>
       <c r="R25" t="str">
-        <f t="shared" si="6"/>
-        <v>key: 'sv':'0'</v>
+        <f t="shared" si="7"/>
+        <v>sv:'0',</v>
       </c>
       <c r="S25" t="str">
-        <f t="shared" si="6"/>
-        <v>{title: 'SV',dataIndex: 'sv',key: 'sv'},:'0'</v>
+        <f t="shared" si="7"/>
+        <v>sv:'0',</v>
       </c>
       <c r="T25" t="str">
-        <f t="shared" si="6"/>
-        <v>:'0'</v>
+        <f t="shared" si="7"/>
+        <v>sv:'0',</v>
       </c>
       <c r="U25" t="str">
-        <f t="shared" si="6"/>
-        <v>:'0'</v>
+        <f t="shared" si="7"/>
+        <v>sv:'0',</v>
       </c>
       <c r="V25" t="str">
-        <f t="shared" si="6"/>
-        <v>:'0'</v>
+        <f t="shared" si="7"/>
+        <v>sv:'0',</v>
       </c>
       <c r="W25" t="str">
-        <f t="shared" si="6"/>
-        <v>:'0'</v>
+        <f t="shared" si="7"/>
+        <v>sv:'0',</v>
       </c>
       <c r="X25" t="str">
-        <f t="shared" si="6"/>
-        <v>:'0'</v>
+        <f t="shared" si="7"/>
+        <v>sv:'0',</v>
       </c>
       <c r="Y25" t="str">
-        <f t="shared" si="6"/>
-        <v>:'0'</v>
+        <f t="shared" si="7"/>
+        <v>sv:'0',</v>
       </c>
       <c r="Z25" t="str">
-        <f t="shared" si="6"/>
-        <v>:'0'</v>
+        <f t="shared" si="7"/>
+        <v>sv:'0',</v>
       </c>
     </row>
     <row r="26" spans="14:26" x14ac:dyDescent="0.2">
       <c r="N26" t="str">
         <f t="shared" si="7"/>
-        <v>cpi:'0.764533640401382'</v>
+        <v>cpi:'0.764533640401382',</v>
       </c>
       <c r="O26" t="str">
-        <f t="shared" si="6"/>
-        <v>CPI:'1.11753458553594'</v>
+        <f t="shared" si="7"/>
+        <v>cpi:'1.11753458553594',</v>
       </c>
       <c r="P26" t="str">
-        <f t="shared" si="6"/>
-        <v>title: 'CPI',:'1.43169771713461'</v>
+        <f t="shared" si="7"/>
+        <v>cpi:'1.43169771713461',</v>
       </c>
       <c r="Q26" t="str">
-        <f t="shared" si="6"/>
-        <v>dataIndex: 'cpi',:'0.765756985055231'</v>
+        <f t="shared" si="7"/>
+        <v>cpi:'0.765756985055231',</v>
       </c>
       <c r="R26" t="str">
-        <f t="shared" si="6"/>
-        <v>key: 'cpi':'1.41853114347691'</v>
+        <f t="shared" si="7"/>
+        <v>cpi:'1.41853114347691',</v>
       </c>
       <c r="S26" t="str">
-        <f t="shared" si="6"/>
-        <v>{title: 'CPI',dataIndex: 'cpi',key: 'cpi'},:'0.734670216420474'</v>
+        <f t="shared" si="7"/>
+        <v>cpi:'0.734670216420474',</v>
       </c>
       <c r="T26" t="str">
-        <f t="shared" si="6"/>
-        <v>:'1.29122848246284'</v>
+        <f t="shared" si="7"/>
+        <v>cpi:'1.29122848246284',</v>
       </c>
       <c r="U26" t="str">
-        <f t="shared" si="6"/>
-        <v>:'0.889497610444108'</v>
+        <f t="shared" si="7"/>
+        <v>cpi:'0.889497610444108',</v>
       </c>
       <c r="V26" t="str">
-        <f t="shared" si="6"/>
-        <v>:'1.64373873249203'</v>
+        <f t="shared" si="7"/>
+        <v>cpi:'1.64373873249203',</v>
       </c>
       <c r="W26" t="str">
-        <f t="shared" si="6"/>
-        <v>:'0.624468085106383'</v>
+        <f t="shared" si="7"/>
+        <v>cpi:'0.624468085106383',</v>
       </c>
       <c r="X26" t="str">
-        <f t="shared" si="6"/>
-        <v>:'1.0824400355345'</v>
+        <f t="shared" si="7"/>
+        <v>cpi:'1.0824400355345',</v>
       </c>
       <c r="Y26" t="str">
-        <f t="shared" si="6"/>
-        <v>:'1.23666412130468'</v>
+        <f t="shared" si="7"/>
+        <v>cpi:'1.23666412130468',</v>
       </c>
       <c r="Z26" t="str">
-        <f t="shared" si="6"/>
-        <v>:'0.791515710427508'</v>
+        <f t="shared" si="7"/>
+        <v>cpi:'0.791515710427508',</v>
       </c>
     </row>
     <row r="27" spans="14:26" x14ac:dyDescent="0.2">
       <c r="N27" t="str">
         <f t="shared" si="7"/>
-        <v>spi:'1'</v>
+        <v>spi:'1',</v>
       </c>
       <c r="O27" t="str">
-        <f t="shared" si="6"/>
-        <v>SPI:'1'</v>
+        <f t="shared" si="7"/>
+        <v>spi:'1',</v>
       </c>
       <c r="P27" t="str">
-        <f t="shared" si="6"/>
-        <v>title: 'SPI',:'1'</v>
+        <f t="shared" si="7"/>
+        <v>spi:'1',</v>
       </c>
       <c r="Q27" t="str">
-        <f t="shared" si="6"/>
-        <v>dataIndex: 'spi',:'1'</v>
+        <f t="shared" si="7"/>
+        <v>spi:'1',</v>
       </c>
       <c r="R27" t="str">
-        <f t="shared" si="6"/>
-        <v>key: 'spi':'1'</v>
+        <f t="shared" si="7"/>
+        <v>spi:'1',</v>
       </c>
       <c r="S27" t="str">
-        <f t="shared" si="6"/>
-        <v>{title: 'SPI',dataIndex: 'spi',key: 'spi'},:'1'</v>
+        <f t="shared" si="7"/>
+        <v>spi:'1',</v>
       </c>
       <c r="T27" t="str">
-        <f t="shared" si="6"/>
-        <v>:'1'</v>
+        <f t="shared" si="7"/>
+        <v>spi:'1',</v>
       </c>
       <c r="U27" t="str">
-        <f t="shared" si="6"/>
-        <v>:'1'</v>
+        <f t="shared" si="7"/>
+        <v>spi:'1',</v>
       </c>
       <c r="V27" t="str">
-        <f t="shared" si="6"/>
-        <v>:'1'</v>
+        <f t="shared" si="7"/>
+        <v>spi:'1',</v>
       </c>
       <c r="W27" t="str">
-        <f t="shared" si="6"/>
-        <v>:'1'</v>
+        <f t="shared" si="7"/>
+        <v>spi:'1',</v>
       </c>
       <c r="X27" t="str">
-        <f t="shared" si="6"/>
-        <v>:'1'</v>
+        <f t="shared" si="7"/>
+        <v>spi:'1',</v>
       </c>
       <c r="Y27" t="str">
-        <f t="shared" si="6"/>
-        <v>:'1'</v>
+        <f t="shared" si="7"/>
+        <v>spi:'1',</v>
       </c>
       <c r="Z27" t="str">
-        <f t="shared" si="6"/>
-        <v>:'1'</v>
+        <f t="shared" si="7"/>
+        <v>spi:'1',</v>
       </c>
     </row>
     <row r="28" spans="14:26" x14ac:dyDescent="0.2">
       <c r="N28" t="str">
         <f t="shared" si="7"/>
-        <v>eac:'3039.5'</v>
+        <v>eac:'3039.5',</v>
       </c>
       <c r="O28" t="str">
-        <f t="shared" si="6"/>
-        <v>EAC:'1778.2'</v>
+        <f t="shared" si="7"/>
+        <v>eac:'1778.2',</v>
       </c>
       <c r="P28" t="str">
-        <f t="shared" si="6"/>
-        <v>title: 'EAC',:'1905.5'</v>
+        <f t="shared" si="7"/>
+        <v>eac:'1905.5',</v>
       </c>
       <c r="Q28" t="str">
-        <f t="shared" si="6"/>
-        <v>dataIndex: 'eac',:'1231.2'</v>
+        <f t="shared" si="7"/>
+        <v>eac:'1231.2',</v>
       </c>
       <c r="R28" t="str">
-        <f t="shared" si="6"/>
-        <v>key: 'eac':'1613.5'</v>
+        <f t="shared" si="7"/>
+        <v>eac:'1613.5',</v>
       </c>
       <c r="S28" t="str">
-        <f t="shared" si="6"/>
-        <v>{title: 'EAC',dataIndex: 'eac',key: 'eac'},:'2328.8'</v>
+        <f t="shared" si="7"/>
+        <v>eac:'2328.8',</v>
       </c>
       <c r="T28" t="str">
-        <f t="shared" si="6"/>
-        <v>:'1702.1'</v>
+        <f t="shared" si="7"/>
+        <v>eac:'1702.1',</v>
       </c>
       <c r="U28" t="str">
-        <f t="shared" si="6"/>
-        <v>:'3431.6'</v>
+        <f t="shared" si="7"/>
+        <v>eac:'3431.6',</v>
       </c>
       <c r="V28" t="str">
-        <f t="shared" si="6"/>
-        <v>:'721.1'</v>
+        <f t="shared" si="7"/>
+        <v>eac:'721.1',</v>
       </c>
       <c r="W28" t="str">
-        <f t="shared" si="6"/>
-        <v>:'1222'</v>
+        <f t="shared" si="7"/>
+        <v>eac:'1222',</v>
       </c>
       <c r="X28" t="str">
-        <f t="shared" si="6"/>
-        <v>:'1688.5'</v>
+        <f t="shared" si="7"/>
+        <v>eac:'1688.5',</v>
       </c>
       <c r="Y28" t="str">
-        <f t="shared" si="6"/>
-        <v>:'1833.4'</v>
+        <f t="shared" si="7"/>
+        <v>eac:'1833.4',</v>
       </c>
       <c r="Z28" t="str">
-        <f t="shared" si="6"/>
-        <v>:'3036.2'</v>
+        <f t="shared" si="7"/>
+        <v>eac:'3036.2',</v>
       </c>
     </row>
     <row r="29" spans="14:26" x14ac:dyDescent="0.2">
       <c r="N29" t="str">
         <f t="shared" si="7"/>
-        <v>etc:'0'</v>
+        <v>etc:'0',</v>
       </c>
       <c r="O29" t="str">
-        <f t="shared" si="6"/>
-        <v>ETC:'0'</v>
+        <f t="shared" si="7"/>
+        <v>etc:'0',</v>
       </c>
       <c r="P29" t="str">
-        <f t="shared" si="6"/>
-        <v>title: 'ETC',:'0'</v>
+        <f t="shared" si="7"/>
+        <v>etc:'0',</v>
       </c>
       <c r="Q29" t="str">
-        <f t="shared" si="6"/>
-        <v>dataIndex: 'etc',:'0'</v>
+        <f t="shared" si="7"/>
+        <v>etc:'0',</v>
       </c>
       <c r="R29" t="str">
-        <f t="shared" si="6"/>
-        <v>key: 'etc':'0'</v>
+        <f t="shared" si="7"/>
+        <v>etc:'0',</v>
       </c>
       <c r="S29" t="str">
-        <f t="shared" si="6"/>
-        <v>{title: 'ETC',dataIndex: 'etc',key: 'etc'},:'0'</v>
+        <f t="shared" si="7"/>
+        <v>etc:'0',</v>
       </c>
       <c r="T29" t="str">
-        <f t="shared" si="6"/>
-        <v>:'0'</v>
+        <f t="shared" si="7"/>
+        <v>etc:'0',</v>
       </c>
       <c r="U29" t="str">
-        <f t="shared" si="6"/>
-        <v>:'0'</v>
+        <f t="shared" si="7"/>
+        <v>etc:'0',</v>
       </c>
       <c r="V29" t="str">
-        <f t="shared" si="6"/>
-        <v>:'0'</v>
+        <f t="shared" si="7"/>
+        <v>etc:'0',</v>
       </c>
       <c r="W29" t="str">
-        <f t="shared" si="6"/>
-        <v>:'0'</v>
+        <f t="shared" si="7"/>
+        <v>etc:'0',</v>
       </c>
       <c r="X29" t="str">
-        <f t="shared" si="6"/>
-        <v>:'0'</v>
+        <f t="shared" si="7"/>
+        <v>etc:'0',</v>
       </c>
       <c r="Y29" t="str">
-        <f t="shared" si="6"/>
-        <v>:'0'</v>
+        <f t="shared" si="7"/>
+        <v>etc:'0',</v>
       </c>
       <c r="Z29" t="str">
-        <f t="shared" si="6"/>
-        <v>:'0'</v>
+        <f t="shared" si="7"/>
+        <v>etc:'0',</v>
       </c>
     </row>
     <row r="30" spans="14:26" x14ac:dyDescent="0.2">
       <c r="N30" t="str">
-        <f>A12&amp;":'"&amp;N12&amp;"'"</f>
-        <v>vac:'-715.7'</v>
+        <f t="shared" si="7"/>
+        <v>vac:'-715.7',</v>
       </c>
       <c r="O30" t="str">
-        <f t="shared" ref="O30:Z33" si="8">B12&amp;":'"&amp;O12&amp;"'"</f>
-        <v>VAC:'209'</v>
+        <f t="shared" si="7"/>
+        <v>vac:'209',</v>
       </c>
       <c r="P30" t="str">
-        <f t="shared" si="8"/>
-        <v>title: 'VAC',:'822.6'</v>
+        <f t="shared" si="7"/>
+        <v>vac:'822.6',</v>
       </c>
       <c r="Q30" t="str">
-        <f t="shared" si="8"/>
-        <v>dataIndex: 'vac',:'-288.4'</v>
+        <f t="shared" si="7"/>
+        <v>vac:'-288.4',</v>
       </c>
       <c r="R30" t="str">
-        <f t="shared" si="8"/>
-        <v>key: 'vac':'675.3'</v>
+        <f t="shared" si="7"/>
+        <v>vac:'675.3',</v>
       </c>
       <c r="S30" t="str">
-        <f t="shared" si="8"/>
-        <v>{title: 'VAC',dataIndex: 'vac',key: 'vac'},:'-617.9'</v>
+        <f t="shared" si="7"/>
+        <v>vac:'-617.9',</v>
       </c>
       <c r="T30" t="str">
-        <f t="shared" si="8"/>
-        <v>:'495.7'</v>
+        <f t="shared" si="7"/>
+        <v>vac:'495.7',</v>
       </c>
       <c r="U30" t="str">
-        <f t="shared" si="8"/>
-        <v>:'-379.2'</v>
+        <f t="shared" si="7"/>
+        <v>vac:'-379.2',</v>
       </c>
       <c r="V30" t="str">
-        <f t="shared" si="8"/>
-        <v>:'464.2'</v>
+        <f t="shared" si="7"/>
+        <v>vac:'464.2',</v>
       </c>
       <c r="W30" t="str">
-        <f t="shared" si="8"/>
-        <v>:'-458.9'</v>
+        <f t="shared" si="7"/>
+        <v>vac:'-458.9',</v>
       </c>
       <c r="X30" t="str">
-        <f t="shared" si="8"/>
-        <v>:'139.2'</v>
+        <f t="shared" si="7"/>
+        <v>vac:'139.2',</v>
       </c>
       <c r="Y30" t="str">
-        <f t="shared" si="8"/>
-        <v>:'433.9'</v>
+        <f t="shared" si="7"/>
+        <v>vac:'433.9',</v>
       </c>
       <c r="Z30" t="str">
-        <f t="shared" si="8"/>
-        <v>:'-633'</v>
+        <f t="shared" si="7"/>
+        <v>vac:'-633',</v>
       </c>
     </row>
     <row r="31" spans="14:26" x14ac:dyDescent="0.2">
       <c r="N31" t="str">
         <f t="shared" si="7"/>
-        <v>plannedProgress    :'1'</v>
+        <v>plannedProgress    :'1',</v>
       </c>
       <c r="O31" t="str">
-        <f t="shared" si="8"/>
-        <v>Planned Progress    :'1'</v>
+        <f t="shared" si="7"/>
+        <v>plannedProgress    :'1',</v>
       </c>
       <c r="P31" t="str">
-        <f t="shared" si="8"/>
-        <v>title: 'Planned Progress    ',:'1'</v>
+        <f t="shared" si="7"/>
+        <v>plannedProgress    :'1',</v>
       </c>
       <c r="Q31" t="str">
-        <f t="shared" si="8"/>
-        <v>dataIndex: 'plannedProgress    ',:'1'</v>
+        <f t="shared" si="7"/>
+        <v>plannedProgress    :'1',</v>
       </c>
       <c r="R31" t="str">
-        <f t="shared" si="8"/>
-        <v>key: 'plannedProgress    ':'1'</v>
+        <f t="shared" si="7"/>
+        <v>plannedProgress    :'1',</v>
       </c>
       <c r="S31" t="str">
-        <f t="shared" si="8"/>
-        <v>{title: 'Planned Progress    ',dataIndex: 'plannedProgress    ',key: 'plannedProgress    '},:'1'</v>
+        <f t="shared" si="7"/>
+        <v>plannedProgress    :'1',</v>
       </c>
       <c r="T31" t="str">
-        <f t="shared" si="8"/>
-        <v>:'1'</v>
+        <f t="shared" si="7"/>
+        <v>plannedProgress    :'1',</v>
       </c>
       <c r="U31" t="str">
-        <f t="shared" si="8"/>
-        <v>:'1'</v>
+        <f t="shared" si="7"/>
+        <v>plannedProgress    :'1',</v>
       </c>
       <c r="V31" t="str">
-        <f t="shared" si="8"/>
-        <v>:'1'</v>
+        <f t="shared" si="7"/>
+        <v>plannedProgress    :'1',</v>
       </c>
       <c r="W31" t="str">
-        <f t="shared" si="8"/>
-        <v>:'1'</v>
+        <f t="shared" si="7"/>
+        <v>plannedProgress    :'1',</v>
       </c>
       <c r="X31" t="str">
-        <f t="shared" si="8"/>
-        <v>:'1'</v>
+        <f t="shared" si="7"/>
+        <v>plannedProgress    :'1',</v>
       </c>
       <c r="Y31" t="str">
-        <f t="shared" si="8"/>
-        <v>:'1'</v>
+        <f t="shared" si="7"/>
+        <v>plannedProgress    :'1',</v>
       </c>
       <c r="Z31" t="str">
-        <f t="shared" si="8"/>
-        <v>:'1'</v>
+        <f t="shared" si="7"/>
+        <v>plannedProgress    :'1',</v>
       </c>
     </row>
     <row r="32" spans="14:26" x14ac:dyDescent="0.2">
       <c r="N32" t="str">
         <f t="shared" si="7"/>
-        <v>actualProgress :'0.9'</v>
+        <v>actualProgress :'0.9',</v>
       </c>
       <c r="O32" t="str">
-        <f t="shared" si="8"/>
-        <v>Actual Progress :'0.9'</v>
+        <f t="shared" si="7"/>
+        <v>actualProgress :'0.9',</v>
       </c>
       <c r="P32" t="str">
-        <f t="shared" si="8"/>
-        <v>title: 'Actual Progress ',:'0.9'</v>
+        <f t="shared" si="7"/>
+        <v>actualProgress :'0.9',</v>
       </c>
       <c r="Q32" t="str">
-        <f t="shared" si="8"/>
-        <v>dataIndex: 'actualProgress ',:'0.9'</v>
+        <f t="shared" si="7"/>
+        <v>actualProgress :'0.9',</v>
       </c>
       <c r="R32" t="str">
-        <f t="shared" si="8"/>
-        <v>key: 'actualProgress ':'0.9'</v>
+        <f t="shared" si="7"/>
+        <v>actualProgress :'0.9',</v>
       </c>
       <c r="S32" t="str">
-        <f t="shared" si="8"/>
-        <v>{title: 'Actual Progress ',dataIndex: 'actualProgress ',key: 'actualProgress '},:'0.9'</v>
+        <f t="shared" si="7"/>
+        <v>actualProgress :'0.9',</v>
       </c>
       <c r="T32" t="str">
-        <f t="shared" si="8"/>
-        <v>:'0.9'</v>
+        <f t="shared" si="7"/>
+        <v>actualProgress :'0.9',</v>
       </c>
       <c r="U32" t="str">
-        <f t="shared" si="8"/>
-        <v>:'0.9'</v>
+        <f t="shared" si="7"/>
+        <v>actualProgress :'0.9',</v>
       </c>
       <c r="V32" t="str">
-        <f t="shared" si="8"/>
-        <v>:'0.9'</v>
+        <f t="shared" si="7"/>
+        <v>actualProgress :'0.9',</v>
       </c>
       <c r="W32" t="str">
-        <f t="shared" si="8"/>
-        <v>:'0.9'</v>
+        <f t="shared" si="7"/>
+        <v>actualProgress :'0.9',</v>
       </c>
       <c r="X32" t="str">
-        <f t="shared" si="8"/>
-        <v>:'0.9'</v>
+        <f t="shared" si="7"/>
+        <v>actualProgress :'0.9',</v>
       </c>
       <c r="Y32" t="str">
-        <f t="shared" si="8"/>
-        <v>:'0.9'</v>
+        <f t="shared" si="7"/>
+        <v>actualProgress :'0.9',</v>
       </c>
       <c r="Z32" t="str">
-        <f t="shared" si="8"/>
-        <v>:'0.9'</v>
+        <f t="shared" si="7"/>
+        <v>actualProgress :'0.9',</v>
       </c>
     </row>
     <row r="33" spans="14:26" x14ac:dyDescent="0.2">
       <c r="N33" t="str">
         <f t="shared" si="7"/>
-        <v>progressDelay:'0.1'</v>
+        <v>progressDelay:'0.1',</v>
       </c>
       <c r="O33" t="str">
-        <f t="shared" si="8"/>
-        <v>Progress Delay:'0.1'</v>
+        <f t="shared" si="7"/>
+        <v>progressDelay:'0.1',</v>
       </c>
       <c r="P33" t="str">
-        <f t="shared" si="8"/>
-        <v>title: 'Progress Delay',:'0.1'</v>
+        <f t="shared" si="7"/>
+        <v>progressDelay:'0.1',</v>
       </c>
       <c r="Q33" t="str">
-        <f t="shared" si="8"/>
-        <v>dataIndex: 'progressDelay',:'0.1'</v>
+        <f t="shared" si="7"/>
+        <v>progressDelay:'0.1',</v>
       </c>
       <c r="R33" t="str">
-        <f t="shared" si="8"/>
-        <v>key: 'progressDelay':'0.1'</v>
+        <f t="shared" si="7"/>
+        <v>progressDelay:'0.1',</v>
       </c>
       <c r="S33" t="str">
-        <f t="shared" si="8"/>
-        <v>{title: 'Progress Delay',dataIndex: 'progressDelay',key: 'progressDelay'},:'0.1'</v>
+        <f t="shared" si="7"/>
+        <v>progressDelay:'0.1',</v>
       </c>
       <c r="T33" t="str">
-        <f t="shared" si="8"/>
-        <v>:'0.1'</v>
+        <f t="shared" si="7"/>
+        <v>progressDelay:'0.1',</v>
       </c>
       <c r="U33" t="str">
-        <f t="shared" si="8"/>
-        <v>:'0.1'</v>
+        <f t="shared" si="7"/>
+        <v>progressDelay:'0.1',</v>
       </c>
       <c r="V33" t="str">
-        <f t="shared" si="8"/>
-        <v>:'0.1'</v>
+        <f t="shared" si="7"/>
+        <v>progressDelay:'0.1',</v>
       </c>
       <c r="W33" t="str">
-        <f t="shared" si="8"/>
-        <v>:'0.1'</v>
+        <f t="shared" si="7"/>
+        <v>progressDelay:'0.1',</v>
       </c>
       <c r="X33" t="str">
-        <f t="shared" si="8"/>
-        <v>:'0.1'</v>
+        <f t="shared" si="7"/>
+        <v>progressDelay:'0.1',</v>
       </c>
       <c r="Y33" t="str">
-        <f t="shared" si="8"/>
-        <v>:'0.1'</v>
+        <f t="shared" si="7"/>
+        <v>progressDelay:'0.1',</v>
       </c>
       <c r="Z33" t="str">
-        <f t="shared" si="8"/>
-        <v>:'0.1'</v>
+        <f t="shared" si="7"/>
+        <v>progressDelay:'0.1',</v>
       </c>
     </row>
   </sheetData>

</xml_diff>